<commit_message>
data processing script completed
</commit_message>
<xml_diff>
--- a/eumf_forecast/keywords/keywords-prototype-21-04-22.xlsx
+++ b/eumf_forecast/keywords/keywords-prototype-21-04-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\stei509\eu_migration_forecast\eumf_forecast\keywords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55AA83B-6CB9-4DC9-9580-248EE4A485F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB42059-98F7-4EBD-B552-F4572159E935}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14670,8 +14670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X2778"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.5" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -33488,21 +33488,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FE58DD3215D6B649BA36E2AB7D5CE029" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4de676c7969066fb6acc5279e215ccc4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="44b7c86c-9f08-4588-83e5-8ab082128caf" xmlns:ns3="943237a1-0af7-4897-9b3f-c25a1fd47b86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b9c23ade8a11b7bc110341a934bc913" ns2:_="" ns3:_="">
     <xsd:import namespace="44b7c86c-9f08-4588-83e5-8ab082128caf"/>
@@ -33713,24 +33698,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90FC0739-CFA1-44B8-9069-C7EA2DEDA71C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747AA91-A9A1-4AB7-BF3B-C9E52BCC4C53}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7415C129-986D-4163-B55B-A8765D8AAD72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33747,4 +33730,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3747AA91-A9A1-4AB7-BF3B-C9E52BCC4C53}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90FC0739-CFA1-44B8-9069-C7EA2DEDA71C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>